<commit_message>
optimize and autonomously pick appliances
</commit_message>
<xml_diff>
--- a/examples/StorageTechnologies_Database.xlsx
+++ b/examples/StorageTechnologies_Database.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiassteggemann/house-energy-mgmt-py/examples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636ECAD9-7B67-A743-8D2A-A9B88E7123A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="780" yWindow="500" windowWidth="13780" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Batteries" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Hydrogen" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Tank" sheetId="3" r:id="rId6"/>
+    <sheet name="Batteries" sheetId="1" r:id="rId1"/>
+    <sheet name="Hydrogen" sheetId="2" r:id="rId2"/>
+    <sheet name="Tank" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -132,59 +141,65 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF0D1F3A"/>
       <name val="HelveticaNeue"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Lora"/>
     </font>
     <font>
       <b/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="7.0"/>
+      <sz val="7"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -194,7 +209,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -204,70 +219,49 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -457,24 +451,30 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="61.29"/>
-    <col customWidth="1" min="4" max="4" width="31.29"/>
+    <col min="1" max="1" width="61.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,41 +497,41 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2">
-        <v>120.0</v>
+        <v>120</v>
       </c>
       <c r="D2" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2">
         <v>0.95</v>
       </c>
       <c r="F2" s="2">
-        <v>239.0</v>
+        <v>239</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2">
-        <v>240.0</v>
+        <v>240</v>
       </c>
       <c r="D3" s="2">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="E3" s="2">
         <v>0.95</v>
@@ -543,15 +543,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2">
         <v>3.6</v>
@@ -560,44 +560,44 @@
         <v>0.95</v>
       </c>
       <c r="F4" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>125.0</v>
+        <v>125</v>
       </c>
       <c r="D5" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="E5" s="2">
         <v>0.95</v>
       </c>
       <c r="F5" s="2">
-        <v>300.0</v>
+        <v>300</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="D6" s="2">
         <v>19.5</v>
@@ -612,18 +612,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2">
         <v>0.95</v>
@@ -637,31 +637,35 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G2"/>
-    <hyperlink r:id="rId2" ref="G3"/>
-    <hyperlink r:id="rId3" ref="G4"/>
-    <hyperlink r:id="rId4" ref="G5"/>
-    <hyperlink r:id="rId5" ref="G6"/>
-    <hyperlink r:id="rId6" ref="G7"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
-  <drawing r:id="rId7"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="35.43"/>
+    <col min="1" max="1" width="35.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -681,21 +685,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2">
         <v>0.5</v>
       </c>
       <c r="E2" s="8">
-        <v>22800.0</v>
+        <v>22800</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>23</v>
@@ -703,26 +707,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="62.43"/>
+    <col min="1" max="1" width="62.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -742,35 +747,35 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="2">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="C2" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2">
         <v>0.9</v>
       </c>
       <c r="E2" s="2">
-        <v>799.0</v>
+        <v>799</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="2">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="C3" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2">
         <v>0.9</v>
@@ -782,15 +787,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="C4" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2">
         <v>0.9</v>
@@ -802,35 +807,35 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="16">
       <c r="A5" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="2">
-        <v>80.0</v>
+        <v>80</v>
       </c>
       <c r="C5" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2">
         <v>0.9</v>
       </c>
       <c r="E5" s="2">
-        <v>399.0</v>
+        <v>399</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="9" t="s">
         <v>34</v>
       </c>
       <c r="B6" s="2">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="C6" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2">
         <v>0.9</v>
@@ -842,21 +847,21 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="C7" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2">
         <v>0.9</v>
       </c>
       <c r="E7" s="2">
-        <v>230.0</v>
+        <v>230</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>37</v>
@@ -864,13 +869,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2"/>
-    <hyperlink r:id="rId2" ref="F3"/>
-    <hyperlink r:id="rId3" ref="F4"/>
-    <hyperlink r:id="rId4" ref="F5"/>
-    <hyperlink r:id="rId5" ref="F6"/>
-    <hyperlink r:id="rId6" ref="F7"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
   </hyperlinks>
-  <drawing r:id="rId7"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>